<commit_message>
add hat v1 notes
</commit_message>
<xml_diff>
--- a/bom/hdmi-board-parts.xlsx
+++ b/bom/hdmi-board-parts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mwg/code/EE Projects 2022-/Homebrew-ECP5-SBC/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2533B0A9-105E-2A4B-ACF4-D44087654915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04932949-0B78-844A-82EB-A0479B8F54BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="2300" windowWidth="36000" windowHeight="22100" xr2:uid="{8691CECE-43C8-1F4A-B1BA-8A041DF9A705}"/>
   </bookViews>
@@ -2448,7 +2448,7 @@
   <dimension ref="A1:O293"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A253" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A268" sqref="A268"/>
+      <selection activeCell="A265" sqref="A265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
reflect addl order of forgotten motherboard parts
</commit_message>
<xml_diff>
--- a/bom/hdmi-board-parts.xlsx
+++ b/bom/hdmi-board-parts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mwg/code/EE Projects 2022-/Homebrew-ECP5-SBC/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6553A607-907C-EC4A-9462-9B7CA51C50CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0198EAB0-7722-AC40-B2D6-A7ED47137497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="2300" windowWidth="36000" windowHeight="22100" xr2:uid="{8691CECE-43C8-1F4A-B1BA-8A041DF9A705}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1304" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="625">
   <si>
     <t>Desc</t>
   </si>
@@ -1931,6 +1931,9 @@
   </si>
   <si>
     <t>R1,R2,R3,R4,R5,R6,R7,R8,R9,R10,R11,R12,R13,R14,R15,R16,R17,R18,R19,R20</t>
+  </si>
+  <si>
+    <t>S1,S2,S3,S4</t>
   </si>
 </sst>
 </file>
@@ -2446,8 +2449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DDB976E-C380-9A4A-ACD0-2206240D942C}">
   <dimension ref="A1:O293"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J262" sqref="J262"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4666,30 +4669,35 @@
         <v>257</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>262</v>
       </c>
-      <c r="D60" t="str">
+      <c r="B60" s="14" t="s">
+        <v>565</v>
+      </c>
+      <c r="D60">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="E60">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G60" s="17" t="str">
+        <v>2</v>
+      </c>
+      <c r="G60" s="17">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="H60" s="9">
         <v>0.27</v>
       </c>
       <c r="I60" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J60" s="4"/>
+        <v>0.54</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="K60" s="7" t="s">
         <v>261</v>
       </c>
@@ -4700,30 +4708,35 @@
         <v>260</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>265</v>
       </c>
-      <c r="D61" t="str">
+      <c r="B61" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="D61">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="E61">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G61" s="17" t="str">
+        <v>2</v>
+      </c>
+      <c r="G61" s="17">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="H61" s="9">
         <v>0.16</v>
       </c>
       <c r="I61" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J61" s="4"/>
+        <v>0.32</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="K61" s="7" t="s">
         <v>264</v>
       </c>
@@ -4734,30 +4747,38 @@
         <v>263</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>266</v>
       </c>
-      <c r="D62" t="str">
+      <c r="B62" s="14" t="s">
+        <v>624</v>
+      </c>
+      <c r="D62">
         <f t="shared" si="0"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="E62">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G62" s="17" t="str">
+        <v>8</v>
+      </c>
+      <c r="F62">
+        <v>12</v>
+      </c>
+      <c r="G62" s="17">
         <f t="shared" si="2"/>
-        <v/>
+        <v>12</v>
       </c>
       <c r="H62" s="9">
         <v>0.4</v>
       </c>
       <c r="I62" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J62" s="4"/>
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="K62" s="7" t="s">
         <v>269</v>
       </c>

</xml_diff>

<commit_message>
correct some bom designators
</commit_message>
<xml_diff>
--- a/bom/hdmi-board-parts.xlsx
+++ b/bom/hdmi-board-parts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mwg/code/EE Projects 2022-/Homebrew-ECP5-SBC/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0198EAB0-7722-AC40-B2D6-A7ED47137497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4ECA41D-068C-0C46-AA8F-D8886CB366B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="2300" windowWidth="36000" windowHeight="22100" xr2:uid="{8691CECE-43C8-1F4A-B1BA-8A041DF9A705}"/>
   </bookViews>
@@ -988,18 +988,12 @@
     <t>C12,C13</t>
   </si>
   <si>
-    <t>C4,C6,C8,C10,C18,C19,C20,C21,C22,C23,C24,C14,C16</t>
-  </si>
-  <si>
     <t>FB2,FB3</t>
   </si>
   <si>
     <t>FB4,FB5,FB6</t>
   </si>
   <si>
-    <t>R43,R56,R60,R63,R64</t>
-  </si>
-  <si>
     <t>R65</t>
   </si>
   <si>
@@ -1030,9 +1024,6 @@
     <t>D7</t>
   </si>
   <si>
-    <t>R45,R46,R68</t>
-  </si>
-  <si>
     <t>0.1" male pins, straight, 2x2</t>
   </si>
   <si>
@@ -1934,6 +1925,15 @@
   </si>
   <si>
     <t>S1,S2,S3,S4</t>
+  </si>
+  <si>
+    <t>C4,C6,C8,C10,C18,C19,C20,C21,C22,C23,C24,C14,C15,C16</t>
+  </si>
+  <si>
+    <t>R45,R48,R49,R46,R68</t>
+  </si>
+  <si>
+    <t>R43,R56,R57,R60,R63,R64</t>
   </si>
 </sst>
 </file>
@@ -2449,8 +2449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DDB976E-C380-9A4A-ACD0-2206240D942C}">
   <dimension ref="A1:O293"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2767,7 +2767,7 @@
         <v>133</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
@@ -2801,31 +2801,31 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>47</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>312</v>
+        <v>624</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G13" s="17">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H13" s="10">
         <v>0.1</v>
       </c>
       <c r="I13" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>1.2000000000000002</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>13</v>
@@ -2952,26 +2952,26 @@
         <v>34</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>323</v>
+        <v>623</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G17" s="17">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H17" s="2">
         <v>1.3299999999999999E-2</v>
       </c>
       <c r="I17" s="3">
         <f t="shared" si="3"/>
-        <v>7.9799999999999996E-2</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>13</v>
@@ -3030,7 +3030,7 @@
         <v>28</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
@@ -3220,7 +3220,7 @@
         <v>40</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
@@ -3298,7 +3298,7 @@
         <v>174</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
@@ -3454,26 +3454,26 @@
         <v>131</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>309</v>
+        <v>622</v>
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E30">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G30" s="17">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H30" s="10">
         <v>0.08</v>
       </c>
       <c r="I30" s="3">
         <f t="shared" si="3"/>
-        <v>2.08</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>13</v>
@@ -3563,7 +3563,7 @@
     </row>
     <row r="33" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B33" s="14" t="s">
         <v>308</v>
@@ -3591,13 +3591,13 @@
         <v>13</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="L33" t="s">
         <v>150</v>
       </c>
       <c r="M33" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -3605,7 +3605,7 @@
         <v>59</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D34">
         <f t="shared" si="0"/>
@@ -3669,13 +3669,13 @@
         <v>13</v>
       </c>
       <c r="K35" s="7" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="L35" t="s">
         <v>96</v>
       </c>
       <c r="M35" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4065,10 +4065,10 @@
     </row>
     <row r="46" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D46">
         <f t="shared" si="0"/>
@@ -4093,13 +4093,13 @@
         <v>13</v>
       </c>
       <c r="K46" s="7" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="L46" t="s">
         <v>64</v>
       </c>
       <c r="M46" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -4674,7 +4674,7 @@
         <v>262</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D60">
         <f t="shared" si="0"/>
@@ -4752,7 +4752,7 @@
         <v>266</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="D62">
         <f t="shared" si="0"/>
@@ -4950,7 +4950,7 @@
         <v>284</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D67">
         <f t="shared" si="0"/>
@@ -4986,10 +4986,10 @@
     </row>
     <row r="68" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>318</v>
+      </c>
+      <c r="B68" s="14" t="s">
         <v>320</v>
-      </c>
-      <c r="B68" s="14" t="s">
-        <v>322</v>
       </c>
       <c r="D68">
         <f t="shared" si="0"/>
@@ -5014,13 +5014,13 @@
         <v>13</v>
       </c>
       <c r="K68" s="7" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="L68" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M68" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="69" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -5142,7 +5142,7 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D72" t="str">
         <f t="shared" si="0"/>
@@ -5165,21 +5165,21 @@
       </c>
       <c r="J72" s="4"/>
       <c r="K72" s="7" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="L72" t="s">
         <v>86</v>
       </c>
       <c r="M72" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="73" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B73" s="14" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D73">
         <f t="shared" si="0"/>
@@ -5204,21 +5204,21 @@
         <v>13</v>
       </c>
       <c r="K73" s="7" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="L73" t="s">
         <v>86</v>
       </c>
       <c r="M73" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="74" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D74">
         <f t="shared" ref="D74:D81" si="15">IF(LEN(B74)=0,"",LEN(B74)-LEN(SUBSTITUTE(B74,",",""))+1)</f>
@@ -5243,18 +5243,18 @@
         <v>13</v>
       </c>
       <c r="K74" s="7" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="L74" t="s">
         <v>86</v>
       </c>
       <c r="M74" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D75" t="str">
         <f t="shared" si="15"/>
@@ -5277,18 +5277,18 @@
       </c>
       <c r="J75" s="4"/>
       <c r="K75" s="7" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="L75" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="M75" s="12" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D76" t="str">
         <f t="shared" si="15"/>
@@ -5311,18 +5311,18 @@
       </c>
       <c r="J76" s="4"/>
       <c r="K76" s="7" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="L76" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="M76" s="12" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="15"/>
@@ -5345,18 +5345,18 @@
       </c>
       <c r="J77" s="4"/>
       <c r="K77" s="7" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="L77" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="M77" s="12" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="15"/>
@@ -5379,18 +5379,18 @@
       </c>
       <c r="J78" s="4"/>
       <c r="K78" s="7" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="L78" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="M78" s="12" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="15"/>
@@ -5413,21 +5413,21 @@
       </c>
       <c r="J79" s="4"/>
       <c r="K79" s="7" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="L79" t="s">
+        <v>332</v>
+      </c>
+      <c r="M79" s="12" t="s">
         <v>335</v>
-      </c>
-      <c r="M79" s="12" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D80">
         <f t="shared" si="15"/>
@@ -5452,21 +5452,21 @@
         <v>13</v>
       </c>
       <c r="K80" s="7" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="L80" t="s">
         <v>24</v>
       </c>
       <c r="M80" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="81" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D81">
         <f t="shared" si="15"/>
@@ -5491,13 +5491,13 @@
         <v>13</v>
       </c>
       <c r="K81" s="7" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="L81" t="s">
         <v>24</v>
       </c>
       <c r="M81" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
@@ -6548,13 +6548,13 @@
         <v>27</v>
       </c>
       <c r="K112" s="7" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="L112" t="s">
         <v>96</v>
       </c>
       <c r="M112" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.2">
@@ -6920,13 +6920,13 @@
         <v>27</v>
       </c>
       <c r="K122" s="7" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="L122" t="s">
         <v>64</v>
       </c>
       <c r="M122" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="O122" s="7"/>
     </row>
@@ -7362,7 +7362,7 @@
     </row>
     <row r="141" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="I141" s="3"/>
       <c r="J141" s="4"/>
@@ -7421,7 +7421,7 @@
         <v>80</v>
       </c>
       <c r="B144" s="14" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="D144">
         <f t="shared" si="23"/>
@@ -7460,7 +7460,7 @@
         <v>44</v>
       </c>
       <c r="B145" s="14" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="D145">
         <f t="shared" si="23"/>
@@ -7618,7 +7618,7 @@
     </row>
     <row r="150" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="I150" s="3"/>
       <c r="J150" s="4"/>
@@ -7657,7 +7657,7 @@
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D153" t="str">
         <f t="shared" si="23"/>
@@ -7680,13 +7680,13 @@
       </c>
       <c r="J153" s="4"/>
       <c r="K153" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L153" t="s">
         <v>29</v>
       </c>
       <c r="M153" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.2">
@@ -7827,7 +7827,7 @@
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="D158" t="str">
         <f t="shared" ref="D158" si="28">IF(LEN(B158)=0,"",LEN(B158)-LEN(SUBSTITUTE(B158,",",""))+1)</f>
@@ -7850,13 +7850,13 @@
       </c>
       <c r="J158" s="4"/>
       <c r="K158" s="7" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="L158" t="s">
         <v>29</v>
       </c>
       <c r="M158" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="159" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -7864,7 +7864,7 @@
         <v>47</v>
       </c>
       <c r="B159" s="14" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="D159">
         <f t="shared" si="23"/>
@@ -8039,7 +8039,7 @@
         <v>292</v>
       </c>
       <c r="B164" s="14" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D164">
         <f t="shared" ref="D164" si="31">IF(LEN(B164)=0,"",LEN(B164)-LEN(SUBSTITUTE(B164,",",""))+1)</f>
@@ -8064,7 +8064,7 @@
         <v>13</v>
       </c>
       <c r="K164" s="7" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="L164" t="s">
         <v>29</v>
@@ -8075,10 +8075,10 @@
     </row>
     <row r="165" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B165" s="14" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="D165">
         <f t="shared" si="23"/>
@@ -8103,13 +8103,13 @@
         <v>13</v>
       </c>
       <c r="K165" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="L165" t="s">
         <v>29</v>
       </c>
       <c r="M165" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.2">
@@ -8151,7 +8151,7 @@
         <v>171</v>
       </c>
       <c r="B167" s="14" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="D167">
         <f>IF(LEN(B167)=0,"",LEN(B167)-LEN(SUBSTITUTE(B167,",",""))+1)</f>
@@ -8190,7 +8190,7 @@
         <v>125</v>
       </c>
       <c r="B168" s="14" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="D168">
         <f t="shared" si="23"/>
@@ -8260,7 +8260,7 @@
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="D170" t="str">
         <f t="shared" ref="D170:D173" si="34">IF(LEN(B170)=0,"",LEN(B170)-LEN(SUBSTITUTE(B170,",",""))+1)</f>
@@ -8283,18 +8283,18 @@
       </c>
       <c r="J170" s="4"/>
       <c r="K170" s="7" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="L170" t="s">
         <v>29</v>
       </c>
       <c r="M170" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="D171" t="str">
         <f t="shared" si="34"/>
@@ -8317,18 +8317,18 @@
       </c>
       <c r="J171" s="4"/>
       <c r="K171" s="7" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="L171" t="s">
         <v>29</v>
       </c>
       <c r="M171" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A172" s="12" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="D172" t="str">
         <f t="shared" si="34"/>
@@ -8351,18 +8351,18 @@
       </c>
       <c r="J172" s="4"/>
       <c r="K172" s="7" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="L172" t="s">
         <v>29</v>
       </c>
       <c r="M172" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A173" s="12" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="D173" t="str">
         <f t="shared" si="34"/>
@@ -8385,13 +8385,13 @@
       </c>
       <c r="J173" s="4"/>
       <c r="K173" s="7" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="L173" t="s">
         <v>29</v>
       </c>
       <c r="M173" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.2">
@@ -8464,10 +8464,10 @@
     </row>
     <row r="176" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
+        <v>410</v>
+      </c>
+      <c r="B176" s="14" t="s">
         <v>413</v>
-      </c>
-      <c r="B176" s="14" t="s">
-        <v>416</v>
       </c>
       <c r="D176">
         <f t="shared" ref="D176" si="37">IF(LEN(B176)=0,"",LEN(B176)-LEN(SUBSTITUTE(B176,",",""))+1)</f>
@@ -8492,13 +8492,13 @@
         <v>13</v>
       </c>
       <c r="K176" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="L176" t="s">
         <v>29</v>
       </c>
       <c r="M176" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.2">
@@ -8574,7 +8574,7 @@
         <v>131</v>
       </c>
       <c r="B179" s="14" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="D179">
         <f t="shared" si="23"/>
@@ -8678,10 +8678,10 @@
     </row>
     <row r="182" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
+        <v>406</v>
+      </c>
+      <c r="B182" s="14" t="s">
         <v>409</v>
-      </c>
-      <c r="B182" s="14" t="s">
-        <v>412</v>
       </c>
       <c r="D182">
         <f t="shared" si="23"/>
@@ -8706,18 +8706,18 @@
         <v>13</v>
       </c>
       <c r="K182" s="7" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="L182" t="s">
         <v>150</v>
       </c>
       <c r="M182" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D183" t="str">
         <f t="shared" ref="D183" si="42">IF(LEN(B183)=0,"",LEN(B183)-LEN(SUBSTITUTE(B183,",",""))+1)</f>
@@ -8740,13 +8740,13 @@
       </c>
       <c r="J183" s="4"/>
       <c r="K183" s="7" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="L183" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="M183" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.2">
@@ -8785,10 +8785,10 @@
     </row>
     <row r="185" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B185" s="14" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D185">
         <f t="shared" si="23"/>
@@ -8813,13 +8813,13 @@
         <v>13</v>
       </c>
       <c r="K185" s="7" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="L185" t="s">
         <v>42</v>
       </c>
       <c r="M185" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="186" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -8827,7 +8827,7 @@
         <v>97</v>
       </c>
       <c r="B186" s="14" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D186">
         <f t="shared" si="23"/>
@@ -8852,18 +8852,18 @@
         <v>13</v>
       </c>
       <c r="K186" s="7" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="L186" t="s">
         <v>96</v>
       </c>
       <c r="M186" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D187" t="str">
         <f t="shared" si="23"/>
@@ -8886,13 +8886,13 @@
       </c>
       <c r="J187" s="4"/>
       <c r="K187" s="7" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="L187" t="s">
         <v>240</v>
       </c>
       <c r="M187" s="12" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.2">
@@ -8931,7 +8931,7 @@
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="D189" t="str">
         <f t="shared" ref="D189" si="47">IF(LEN(B189)=0,"",LEN(B189)-LEN(SUBSTITUTE(B189,",",""))+1)</f>
@@ -8954,21 +8954,21 @@
       </c>
       <c r="J189" s="4"/>
       <c r="K189" s="7" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="L189" t="s">
         <v>29</v>
       </c>
       <c r="M189" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="190" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B190" s="14" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D190">
         <f t="shared" ref="D190" si="50">IF(LEN(B190)=0,"",LEN(B190)-LEN(SUBSTITUTE(B190,",",""))+1)</f>
@@ -8993,18 +8993,18 @@
         <v>13</v>
       </c>
       <c r="K190" s="7" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="L190" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="M190" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="E191">
         <f t="shared" si="27"/>
@@ -9023,13 +9023,13 @@
       </c>
       <c r="J191" s="4"/>
       <c r="K191" s="7" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="L191" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="M191" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="192" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -9037,7 +9037,7 @@
         <v>270</v>
       </c>
       <c r="B192" s="14" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D192">
         <f t="shared" si="23"/>
@@ -9115,7 +9115,7 @@
         <v>278</v>
       </c>
       <c r="B194" s="14" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D194">
         <f t="shared" si="23"/>
@@ -9224,7 +9224,7 @@
     </row>
     <row r="197" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D197" t="str">
         <f t="shared" si="23"/>
@@ -9247,21 +9247,21 @@
       </c>
       <c r="J197" s="4"/>
       <c r="K197" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="L197" t="s">
+        <v>313</v>
+      </c>
+      <c r="M197" t="s">
         <v>314</v>
-      </c>
-      <c r="L197" t="s">
-        <v>315</v>
-      </c>
-      <c r="M197" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="198" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B198" s="14" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="D198">
         <f t="shared" si="23"/>
@@ -9286,21 +9286,21 @@
         <v>13</v>
       </c>
       <c r="K198" s="7" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="L198" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="M198" s="12" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="199" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B199" s="14" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D199">
         <f t="shared" si="23"/>
@@ -9325,21 +9325,21 @@
         <v>13</v>
       </c>
       <c r="K199" s="7" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="L199" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="M199" s="12" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="200" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B200" s="14" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="D200">
         <f t="shared" si="23"/>
@@ -9364,18 +9364,18 @@
         <v>13</v>
       </c>
       <c r="K200" s="7" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="L200" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="M200" s="12" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="201" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D201" t="str">
         <f t="shared" si="23"/>
@@ -9398,21 +9398,21 @@
       </c>
       <c r="J201" s="4"/>
       <c r="K201" s="7" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="L201" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="M201" s="12" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="202" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B202" s="14" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="D202">
         <f t="shared" si="23"/>
@@ -9437,18 +9437,18 @@
         <v>13</v>
       </c>
       <c r="K202" s="7" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="L202" t="s">
+        <v>332</v>
+      </c>
+      <c r="M202" s="12" t="s">
         <v>335</v>
-      </c>
-      <c r="M202" s="12" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="203" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D203" t="str">
         <f t="shared" si="23"/>
@@ -9471,18 +9471,18 @@
       </c>
       <c r="J203" s="4"/>
       <c r="K203" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="L203" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="M203" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="204" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D204" t="str">
         <f t="shared" si="23"/>
@@ -9505,18 +9505,18 @@
       </c>
       <c r="J204" s="4"/>
       <c r="K204" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="L204" t="s">
         <v>240</v>
       </c>
       <c r="M204" s="12" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="205" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D205" t="str">
         <f t="shared" si="23"/>
@@ -9539,18 +9539,18 @@
       </c>
       <c r="J205" s="4"/>
       <c r="K205" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="L205" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="M205" s="12" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="206" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D206" t="str">
         <f t="shared" si="23"/>
@@ -9573,13 +9573,13 @@
       </c>
       <c r="J206" s="4"/>
       <c r="K206" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="L206" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="M206" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="207" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -9587,7 +9587,7 @@
         <v>80</v>
       </c>
       <c r="B207" s="14" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="D207">
         <f t="shared" ref="D207:D213" si="55">IF(LEN(B207)=0,"",LEN(B207)-LEN(SUBSTITUTE(B207,",",""))+1)</f>
@@ -9735,10 +9735,10 @@
     </row>
     <row r="211" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="B211" s="14" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="D211">
         <f t="shared" ref="D211" si="58">IF(LEN(B211)=0,"",LEN(B211)-LEN(SUBSTITUTE(B211,",",""))+1)</f>
@@ -9763,18 +9763,18 @@
         <v>13</v>
       </c>
       <c r="K211" s="7" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="L211" t="s">
         <v>86</v>
       </c>
       <c r="M211" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="212" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B212" s="14" t="s">
         <v>203</v>
@@ -9813,10 +9813,10 @@
     </row>
     <row r="213" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A213" s="21" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B213" s="14" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="D213">
         <f t="shared" si="55"/>
@@ -9841,21 +9841,21 @@
         <v>13</v>
       </c>
       <c r="K213" s="7" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="L213" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="M213" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="214" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A214" s="21" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="B214" s="14" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="D214">
         <f t="shared" ref="D214" si="65">IF(LEN(B214)=0,"",LEN(B214)-LEN(SUBSTITUTE(B214,",",""))+1)</f>
@@ -9880,18 +9880,18 @@
         <v>13</v>
       </c>
       <c r="K214" s="7" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="L214" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="M214" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="215" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A215" s="21" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="D215" t="str">
         <f t="shared" ref="D215" si="68">IF(LEN(B215)=0,"",LEN(B215)-LEN(SUBSTITUTE(B215,",",""))+1)</f>
@@ -9914,18 +9914,18 @@
       </c>
       <c r="J215" s="4"/>
       <c r="K215" s="7" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="L215" t="s">
         <v>24</v>
       </c>
       <c r="M215" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="216" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A216" s="19" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="H216" s="2"/>
       <c r="I216" s="3"/>
@@ -9934,7 +9934,7 @@
     </row>
     <row r="217" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A217" s="20" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B217" s="14" t="s">
         <v>113</v>
@@ -9962,21 +9962,21 @@
         <v>13</v>
       </c>
       <c r="K217" s="7" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L217" t="s">
         <v>24</v>
       </c>
       <c r="M217" s="18" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="218" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A218" s="20" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="B218" s="14" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="D218">
         <f t="shared" si="71"/>
@@ -10004,21 +10004,21 @@
         <v>13</v>
       </c>
       <c r="K218" s="7" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="L218" t="s">
         <v>42</v>
       </c>
       <c r="M218" s="18" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="219" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A219" s="20" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B219" s="14" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="D219">
         <f t="shared" si="71"/>
@@ -10043,21 +10043,21 @@
         <v>13</v>
       </c>
       <c r="K219" s="7" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="L219" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="M219" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="220" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A220" s="20" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B220" s="14" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="D220">
         <f t="shared" si="71"/>
@@ -10082,21 +10082,21 @@
         <v>13</v>
       </c>
       <c r="K220" s="7" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="L220" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="M220" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="221" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A221" s="20" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B221" s="14" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D221">
         <f t="shared" si="71"/>
@@ -10121,21 +10121,21 @@
         <v>13</v>
       </c>
       <c r="K221" s="7" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="L221" t="s">
         <v>96</v>
       </c>
       <c r="M221" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="222" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A222" s="20" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B222" s="14" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="D222">
         <f t="shared" si="71"/>
@@ -10160,21 +10160,21 @@
         <v>13</v>
       </c>
       <c r="K222" s="7" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L222" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="M222" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="223" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A223" s="20" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B223" s="14" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="D223">
         <f t="shared" si="71"/>
@@ -10199,21 +10199,21 @@
         <v>13</v>
       </c>
       <c r="K223" s="7" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="L223" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="M223" s="18" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="224" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A224" s="20" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B224" s="14" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="D224">
         <f t="shared" si="71"/>
@@ -10238,21 +10238,21 @@
         <v>13</v>
       </c>
       <c r="K224" s="7" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="L224" t="s">
         <v>29</v>
       </c>
       <c r="M224" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="225" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A225" s="20" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B225" s="14" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="D225">
         <f t="shared" si="71"/>
@@ -10277,21 +10277,21 @@
         <v>13</v>
       </c>
       <c r="K225" s="7" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="L225" t="s">
         <v>42</v>
       </c>
       <c r="M225" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="226" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A226" s="20" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B226" s="14" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D226">
         <f t="shared" si="71"/>
@@ -10316,21 +10316,21 @@
         <v>13</v>
       </c>
       <c r="K226" s="7" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="L226" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="M226" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="227" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A227" s="20" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B227" s="14" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="D227">
         <f t="shared" si="71"/>
@@ -10355,21 +10355,21 @@
         <v>13</v>
       </c>
       <c r="K227" s="7" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="L227" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="M227" s="18" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="228" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A228" s="20" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B228" s="14" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="D228">
         <f t="shared" si="71"/>
@@ -10394,21 +10394,21 @@
         <v>13</v>
       </c>
       <c r="K228" s="7" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="L228" t="s">
         <v>29</v>
       </c>
       <c r="M228" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="229" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A229" s="20" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B229" s="14" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="D229">
         <f t="shared" si="71"/>
@@ -10433,21 +10433,21 @@
         <v>13</v>
       </c>
       <c r="K229" s="7" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="L229" t="s">
         <v>29</v>
       </c>
       <c r="M229" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="230" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A230" s="20" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B230" s="14" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D230">
         <f t="shared" si="71"/>
@@ -10472,21 +10472,21 @@
         <v>13</v>
       </c>
       <c r="K230" s="7" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="L230" t="s">
         <v>24</v>
       </c>
       <c r="M230" s="18" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="231" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A231" s="20" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B231" s="14" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="D231">
         <f t="shared" si="71"/>
@@ -10511,21 +10511,21 @@
         <v>13</v>
       </c>
       <c r="K231" s="7" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="L231" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="M231" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="232" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A232" s="20" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B232" s="14" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="D232">
         <f t="shared" si="71"/>
@@ -10550,21 +10550,21 @@
         <v>13</v>
       </c>
       <c r="K232" s="7" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="L232" t="s">
         <v>96</v>
       </c>
       <c r="M232" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="233" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A233" s="20" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="B233" s="14" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="D233">
         <f t="shared" si="71"/>
@@ -10589,21 +10589,21 @@
         <v>13</v>
       </c>
       <c r="K233" s="7" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="L233" t="s">
         <v>29</v>
       </c>
       <c r="M233" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="234" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A234" s="20" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B234" s="14" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="D234">
         <f t="shared" si="71"/>
@@ -10628,21 +10628,21 @@
         <v>13</v>
       </c>
       <c r="K234" s="7" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="L234" t="s">
         <v>96</v>
       </c>
       <c r="M234" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="235" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A235" s="20" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B235" s="14" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D235">
         <f t="shared" si="71"/>
@@ -10667,21 +10667,21 @@
         <v>13</v>
       </c>
       <c r="K235" s="7" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="L235" t="s">
         <v>96</v>
       </c>
       <c r="M235" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="236" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A236" s="20" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B236" s="14" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="D236">
         <f t="shared" si="71"/>
@@ -10706,21 +10706,21 @@
         <v>13</v>
       </c>
       <c r="K236" s="7" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="L236" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="M236" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="237" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A237" s="20" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B237" s="14" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D237">
         <f t="shared" si="71"/>
@@ -10745,18 +10745,18 @@
         <v>13</v>
       </c>
       <c r="K237" s="7" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="L237" t="s">
         <v>29</v>
       </c>
       <c r="M237" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="238" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A238" s="21" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D238" t="str">
         <f t="shared" si="71"/>
@@ -10779,18 +10779,18 @@
       </c>
       <c r="J238" s="4"/>
       <c r="K238" s="7" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="L238" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="M238" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="239" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A239" s="21" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="D239" t="str">
         <f t="shared" ref="D239:D242" si="74">IF(LEN(B239)=0,"",LEN(B239)-LEN(SUBSTITUTE(B239,",",""))+1)</f>
@@ -10813,18 +10813,18 @@
       </c>
       <c r="J239" s="4"/>
       <c r="K239" s="7" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="L239" t="s">
         <v>24</v>
       </c>
       <c r="M239" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="240" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A240" s="21" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="D240" t="str">
         <f t="shared" si="74"/>
@@ -10847,21 +10847,21 @@
       </c>
       <c r="J240" s="4"/>
       <c r="K240" s="7" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="L240" t="s">
         <v>118</v>
       </c>
       <c r="M240" s="12" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="241" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A241" s="21" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B241" s="14" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D241">
         <f t="shared" si="74"/>
@@ -10886,18 +10886,18 @@
         <v>13</v>
       </c>
       <c r="K241" s="7" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="L241" t="s">
         <v>64</v>
       </c>
       <c r="M241" s="12" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="242" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A242" s="21" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="B242" s="14" t="s">
         <v>244</v>
@@ -10925,13 +10925,13 @@
         <v>13</v>
       </c>
       <c r="K242" s="7" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="L242" t="s">
         <v>118</v>
       </c>
       <c r="M242" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="244" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -11177,7 +11177,7 @@
     </row>
     <row r="254" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="B254" s="14" t="s">
         <v>82</v>
@@ -11205,18 +11205,18 @@
         <v>13</v>
       </c>
       <c r="K254" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="L254" t="s">
         <v>42</v>
       </c>
       <c r="M254" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="255" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="B255" s="14" t="s">
         <v>83</v>
@@ -11244,21 +11244,21 @@
         <v>13</v>
       </c>
       <c r="K255" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="L255" t="s">
         <v>42</v>
       </c>
       <c r="M255" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="256" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B256" s="14" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="D256">
         <f t="shared" si="85"/>
@@ -11283,18 +11283,18 @@
         <v>13</v>
       </c>
       <c r="K256" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="L256" t="s">
         <v>29</v>
       </c>
       <c r="M256" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="257" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="D257" t="str">
         <f t="shared" ref="D257" si="88">IF(LEN(B257)=0,"",LEN(B257)-LEN(SUBSTITUTE(B257,",",""))+1)</f>
@@ -11317,21 +11317,21 @@
       </c>
       <c r="J257" s="4"/>
       <c r="K257" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="L257" t="s">
         <v>29</v>
       </c>
       <c r="M257" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="258" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="B258" s="14" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="D258">
         <f t="shared" ref="D258:D259" si="91">IF(LEN(B258)=0,"",LEN(B258)-LEN(SUBSTITUTE(B258,",",""))+1)</f>
@@ -11356,18 +11356,18 @@
         <v>13</v>
       </c>
       <c r="K258" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="L258" t="s">
         <v>29</v>
       </c>
       <c r="M258" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="259" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="D259" t="str">
         <f t="shared" si="91"/>
@@ -11390,18 +11390,18 @@
       </c>
       <c r="J259" s="4"/>
       <c r="K259" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="L259" t="s">
         <v>29</v>
       </c>
       <c r="M259" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="260" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="B260" s="14" t="s">
         <v>12</v>
@@ -11429,18 +11429,18 @@
         <v>13</v>
       </c>
       <c r="K260" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="L260" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="M260" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="261" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="B261" s="14" t="s">
         <v>12</v>
@@ -11468,18 +11468,18 @@
         <v>13</v>
       </c>
       <c r="K261" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="L261" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="M261" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="262" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="B262" s="14" t="s">
         <v>81</v>
@@ -11507,18 +11507,18 @@
         <v>13</v>
       </c>
       <c r="K262" s="7" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="L262" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="M262" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="263" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B263" s="14" t="s">
         <v>93</v>
@@ -11549,13 +11549,13 @@
         <v>13</v>
       </c>
       <c r="K263" s="7" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="L263" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M263" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="264" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -11563,7 +11563,7 @@
         <v>133</v>
       </c>
       <c r="B264" s="14" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="D264">
         <f t="shared" si="94"/>
@@ -11602,7 +11602,7 @@
     </row>
     <row r="265" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="B265" s="14" t="s">
         <v>190</v>
@@ -11630,18 +11630,18 @@
         <v>13</v>
       </c>
       <c r="K265" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="L265" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="M265" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="266" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="B266" s="14" t="s">
         <v>20</v>
@@ -11669,21 +11669,21 @@
         <v>13</v>
       </c>
       <c r="K266" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="L266" t="s">
         <v>24</v>
       </c>
       <c r="M266" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="267" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="B267" s="14" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D267">
         <f t="shared" ref="D267" si="98">IF(LEN(B267)=0,"",LEN(B267)-LEN(SUBSTITUTE(B267,",",""))+1)</f>
@@ -11708,18 +11708,18 @@
         <v>13</v>
       </c>
       <c r="K267" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="L267" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="M267" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="269" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A269" s="5" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="I269" s="3"/>
       <c r="J269" s="4"/>
@@ -11736,7 +11736,7 @@
     </row>
     <row r="271" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D271" t="str">
         <f>IF(LEN(B271)=0,"",LEN(B271)-LEN(SUBSTITUTE(B271,",",""))+1)</f>
@@ -11761,18 +11761,18 @@
         <v>27</v>
       </c>
       <c r="K271" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="L271" t="s">
         <v>64</v>
       </c>
       <c r="M271" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="290" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A290" s="5" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="I290" s="3"/>
       <c r="J290" s="4"/>
@@ -11789,10 +11789,10 @@
     </row>
     <row r="292" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B292" s="14" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D292">
         <f>IF(LEN(B292)=0,"",LEN(B292)-LEN(SUBSTITUTE(B292,",",""))+1)</f>
@@ -11831,10 +11831,10 @@
     </row>
     <row r="293" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B293" s="14" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D293">
         <f>IF(LEN(B293)=0,"",LEN(B293)-LEN(SUBSTITUTE(B293,",",""))+1)</f>
@@ -11862,13 +11862,13 @@
         <v>13</v>
       </c>
       <c r="K293" s="7" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="L293" t="s">
         <v>64</v>
       </c>
       <c r="M293" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>